<commit_message>
here the 50% of lit survey generated -- agent from scratch.
</commit_message>
<xml_diff>
--- a/Agents/literature_survey.xlsx
+++ b/Agents/literature_survey.xlsx
@@ -498,188 +498,192 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2508.04681v1</t>
+          <t>2508.05619v1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Perceiving and Acting in First-Person: A Dataset and Benchmark for
-  Egocentric Human-Object-Human Interactions</t>
+          <t>The Missing Reward: Active Inference in the Era of Experience</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Liang Xu, Chengqun Yang, Zili Lin, Fei Xu, Yifan Liu, Congsheng Xu, Yiyi Zhang, Jie Qin, Xingdong Sheng, Yunhui Liu, Xin Jin, Yichao Yan, Wenjun Zeng, Xiaokang Yang</t>
+          <t>Bo Wen</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://arxiv.org/abs/2508.04681v1</t>
+          <t>http://arxiv.org/abs/2508.05619v1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Learning action models from real-world human-centric interaction datasets is
-important towards building general-purpose intelligent assistants with
-efficiency. However, most existing datasets only offer specialist interaction
-category and ignore that AI assistants perceive and act based on first-person
-acquisition. We urge that both the generalist interaction knowledge and
-egocentric modality are indispensable. In this paper, we embed the
-manual-assisted task into a vision-language-action framework, where the
-assistant provides services to the instructor following egocentric vision and
-commands. With our hybrid RGB-MoCap system, pairs of assistants and instructors
-engage with multiple objects and the scene following GPT-generated scripts.
-Under this setting, we accomplish InterVLA, the first large-scale
-human-object-human interaction dataset with 11.4 hours and 1.2M frames of
-multimodal data, spanning 2 egocentric and 5 exocentric videos, accurate
-human/object motions and verbal commands. Furthermore, we establish novel
-benchmarks on egocentric human motion estimation, interaction synthesis, and
-interaction prediction with comprehensive analysis. We believe that our
-InterVLA testbed and the benchmarks will foster future works on building AI
-agents in the physical world.
+          <t xml:space="preserve">  This paper argues that Active Inference (AIF) provides a crucial foundation
+for developing autonomous AI agents capable of learning from experience without
+continuous human reward engineering. As AI systems begin to exhaust
+high-quality training data and rely on increasingly large human workforces for
+reward design, the current paradigm faces significant scalability challenges
+that could impede progress toward genuinely autonomous intelligence. The
+proposal for an ``Era of Experience,'' where agents learn from self-generated
+data, is a promising step forward. However, this vision still depends on
+extensive human engineering of reward functions, effectively shifting the
+bottleneck from data curation to reward curation. This highlights what we
+identify as the \textbf{grounded-agency gap}: the inability of contemporary AI
+systems to autonomously formulate, adapt, and pursue objectives in response to
+changing circumstances. We propose that AIF can bridge this gap by replacing
+external reward signals with an intrinsic drive to minimize free energy,
+allowing agents to naturally balance exploration and exploitation through a
+unified Bayesian objective. By integrating Large Language Models as generative
+world models with AIF's principled decision-making framework, we can create
+agents that learn efficiently from experience while remaining aligned with
+human values. This synthesis offers a compelling path toward AI systems that
+can develop autonomously while adhering to both computational and physical
+constraints.
 </t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Accepted to ICCV 2025. Project Page:
-  https://liangxuy.github.io/InterVLA/</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- Active Inference (AIF),   - Large Language Models (as generative world models),   - Bayesian objective for balancing exploration and exploitation,   - Free energy minimization, , -</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- AIF provides a foundation for developing autonomous AI agents capable of learning from experience without continuous human reward engineering.,   - AIF can bridge the grounded-agency gap by replacing external reward signals with an intrinsic drive to minimize free energy.,   - Integration of Large Language Models with AIF's decision-making framework can create agents that learn efficiently from experience while remaining aligned with human values.,   - This approach offers a path toward AI systems that can develop autonomously while adhering to computational and physical constraints., , -</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- Current AI systems face significant scalability challenges due to reliance on high-quality training data and extensive human workforces for reward design.,   - The proposed "Era of Experience" still depends on extensive human engineering of reward functions, shifting the bottleneck from data curation to reward curation., , -</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- The grounded-agency gap: the inability of contemporary AI systems to autonomously formulate, adapt, and pursue objectives in response to changing circumstances.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2508.04678v1</t>
+          <t>2508.05614v1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Open Scene Graphs for Open-World Object-Goal Navigation</t>
+          <t>OmniEAR: Benchmarking Agent Reasoning in Embodied Tasks</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Joel Loo, Zhanxin Wu, David Hsu</t>
+          <t>Zixuan Wang, Dingming Li, Hongxing Li, Shuo Chen, Yuchen Yan, Wenqi Zhang, Yongliang Shen, Weiming Lu, Jun Xiao, Yueting Zhuang</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>http://arxiv.org/abs/2508.04678v1</t>
+          <t>http://arxiv.org/abs/2508.05614v1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  How can we build general-purpose robot systems for open-world semantic
-navigation, e.g., searching a novel environment for a target object specified
-in natural language? To tackle this challenge, we introduce OSG Navigator, a
-modular system composed of foundation models, for open-world Object-Goal
-Navigation (ObjectNav). Foundation models provide enormous semantic knowledge
-about the world, but struggle to organise and maintain spatial information
-effectively at scale. Key to OSG Navigator is the Open Scene Graph
-representation, which acts as spatial memory for OSG Navigator. It organises
-spatial information hierarchically using OSG schemas, which are templates, each
-describing the common structure of a class of environments. OSG schemas can be
-automatically generated from simple semantic labels of a given environment,
-e.g., "home" or "supermarket". They enable OSG Navigator to adapt zero-shot to
-new environment types. We conducted experiments using both Fetch and Spot
-robots in simulation and in the real world, showing that OSG Navigator achieves
-state-of-the-art performance on ObjectNav benchmarks and generalises zero-shot
-over diverse goals, environments, and robot embodiments.
+          <t xml:space="preserve">  Large language models excel at abstract reasoning but their capacity for
+embodied agent reasoning remains largely unexplored. We present OmniEAR, a
+comprehensive framework for evaluating how language models reason about
+physical interactions, tool usage, and multi-agent coordination in embodied
+tasks. Unlike existing benchmarks that provide predefined tool sets or explicit
+collaboration directives, OmniEAR requires agents to dynamically acquire
+capabilities and autonomously determine coordination strategies based on task
+demands. Through text-based environment representation, we model continuous
+physical properties and complex spatial relationships across 1,500 scenarios
+spanning household and industrial domains. Our systematic evaluation reveals
+severe performance degradation when models must reason from constraints: while
+achieving 85-96% success with explicit instructions, performance drops to
+56-85% for tool reasoning and 63-85% for implicit collaboration, with compound
+tasks showing over 50% failure rates. Surprisingly, complete environmental
+information degrades coordination performance, indicating models cannot filter
+task-relevant constraints. Fine-tuning improves single-agent tasks dramatically
+(0.6% to 76.3%) but yields minimal multi-agent gains (1.5% to 5.5%), exposing
+fundamental architectural limitations. These findings demonstrate that embodied
+reasoning poses fundamentally different challenges than current models can
+address, establishing OmniEAR as a rigorous benchmark for evaluating and
+advancing embodied AI systems. Our code and data are included in the
+supplementary materials and will be open-sourced upon acceptance.
 </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>In IJRR Special Issue: Foundation Models and Neuro-symbolic AI for
-  Robotics. Journal extension to arXiv:2407.02473</t>
+          <t>Project Page: https://zju-real.github.io/OmniEmbodied Code:
+  https://github.com/ZJU-REAL/OmniEmbodied</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>10.1177/02783649251369549</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- OmniEAR framework,   - Text-based environment representation,   - Fine-tuning of language models,   - Evaluation across 1,500 scenarios spanning household and industrial domains, , -</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- Comprehensive evaluation of language models' reasoning about physical interactions, tool usage, and multi-agent coordination,   - Dynamic acquisition of capabilities and autonomous determination of coordination strategies,   - Systematic evaluation revealing performance insights,   - Establishment of a rigorous benchmark for embodied AI systems,   - Open-sourcing of code and data, , -</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- Severe performance degradation when models must reason from constraints,   - Performance drops significantly for tool reasoning and implicit collaboration tasks,   - High failure rates for compound tasks,   - Degraded coordination performance with complete environmental information,   - Minimal multi-agent gains from fine-tuning, , -</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- The need for improved models that can better handle embodied reasoning tasks,   - The challenge of filtering task-relevant constraints from complete environmental information,   - Fundamental architectural limitations in current models for multi-agent tasks,   - The necessity for further advancements in embodied AI systems to address the unique challenges posed by embodied reasoning</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2508.04660v1</t>
+          <t>2508.05519v1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Multi-module GRPO: Composing Policy Gradients and Prompt Optimization
-  for Language Model Programs</t>
+          <t>Leveraging AI to Accelerate Clinical Data Cleaning: A Comparative Study
+  of AI-Assisted vs. Traditional Methods</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Noah Ziems, Dilara Soylu, Lakshya A Agrawal, Isaac Miller, Liheng Lai, Chen Qian, Kaiqiang Song, Meng Jiang, Dan Klein, Matei Zaharia, Karel D'Oosterlinck, Christopher Potts, Omar Khattab</t>
+          <t>Matthew Purri, Amit Patel, Erik Deurrell</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>http://arxiv.org/abs/2508.04660v1</t>
+          <t>http://arxiv.org/abs/2508.05519v1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Group Relative Policy Optimization (GRPO) has proven to be an effective tool
-for post-training language models (LMs). However, AI systems are increasingly
-expressed as modular programs that mix together multiple LM calls with distinct
-prompt templates and other tools, and it is not clear how best to leverage GRPO
-to improve these systems. We begin to address this challenge by defining
-mmGRPO, a simple multi-module generalization of GRPO that groups LM calls by
-module across rollouts and handles variable-length and interrupted
-trajectories. We find that mmGRPO, composed with automatic prompt optimization,
-improves accuracy by 11% on average across classification, many-hop search, and
-privacy-preserving delegation tasks against the post-trained LM, and by 5%
-against prompt optimization on its own. We open-source mmGRPO in DSPy as the
-dspy.GRPO optimizer.
+          <t xml:space="preserve">  Clinical trial data cleaning represents a critical bottleneck in drug
+development, with manual review processes struggling to manage exponentially
+increasing data volumes and complexity. This paper presents Octozi, an
+artificial intelligence-assisted platform that combines large language models
+with domain-specific heuristics to transform clinical data review. In a
+controlled experimental study with experienced clinical reviewers (n=10), we
+demonstrate that AI assistance increased data cleaning throughput by 6.03-fold
+while simultaneously decreasing cleaning errors from 54.67% to 8.48% (a
+6.44-fold improvement). Crucially, the system reduced false positive queries by
+15.48-fold, minimizing unnecessary site burden. These improvements were
+consistent across reviewers regardless of experience level, suggesting broad
+applicability. Our findings indicate that AI-assisted approaches can address
+fundamental inefficiencies in clinical trial operations, potentially
+accelerating drug development timelines and reducing costs while maintaining
+regulatory compliance. This work establishes a framework for integrating AI
+into safety-critical clinical workflows and demonstrates the transformative
+potential of human-AI collaboration in pharmaceutical clinical trials.
 </t>
         </is>
       </c>
@@ -688,68 +692,72 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- Artificial Intelligence (AI)-assisted platform: Octozi,   - Large language models,   - Domain-specific heuristics,   - Controlled experimental study with experienced clinical reviewers (n=10), , -</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- Increased data cleaning throughput by 6.03-fold,   - Decreased cleaning errors from 54.67% to 8.48% (a 6.44-fold improvement),   - Reduced false positive queries by 15.48-fold, minimizing unnecessary site burden,   - Consistent improvements across reviewers regardless of experience level,   - Potential to accelerate drug development timelines and reduce costs,   - Maintained regulatory compliance, , -</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- The study's sample size is relatively small (n=10), which may not represent the entire population of clinical reviewers.,   - The abstract does not mention any potential drawbacks or challenges of implementing the AI-assisted platform in real-world settings.,   - The long-term effects and adaptability of the AI system to evolving clinical trial data and protocols are not discussed., , -</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Not available</t>
+          <t>- The abstract does not provide information on how the AI system handles different types of clinical trial data or its adaptability to various trial phases.,   - There is no mention of how the AI system ensures data privacy and security, which is crucial in clinical trials.,   - The abstract does not discuss the potential for bias in the AI system and how it is addressed.,   - Further research is needed to evaluate the system's performance in diverse clinical trial settings and with larger groups of reviewers.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2508.04658v1</t>
+          <t>2508.05469v1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>YOLOv8-Based Deep Learning Model for Automated Poultry Disease Detection
-  and Health Monitoring paper</t>
+          <t>Let's Measure Information Step-by-Step: LLM-Based Evaluation Beyond
+  Vibes</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Akhil Saketh Reddy Sabbella, Ch. Lakshmi Prachothan, Eswar Kumar Panta</t>
+          <t>Zachary Robertson, Sanmi Koyejo</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>http://arxiv.org/abs/2508.04658v1</t>
+          <t>http://arxiv.org/abs/2508.05469v1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  In the poultry industry, detecting chicken illnesses is essential to avoid
-financial losses. Conventional techniques depend on manual observation, which
-is laborious and prone to mistakes. Using YOLO v8 a deep learning model for
-real-time object recognition. This study suggests an AI based approach, by
-developing a system that analyzes high resolution chicken photos, YOLO v8
-detects signs of illness, such as abnormalities in behavior and appearance. A
-sizable, annotated dataset has been used to train the algorithm, which provides
-accurate real-time identification of infected chicken and prompt warnings to
-farm operators for prompt action. By facilitating early infection
-identification, eliminating the need for human inspection, and enhancing
-biosecurity in large-scale farms, this AI technology improves chicken health
-management. The real-time features of YOLO v8 provide a scalable and effective
-method for improving farm management techniques.
+          <t xml:space="preserve">  We develop mechanisms for evaluating AI systems without ground truth by
+exploiting a connection between gaming resistance and output quality. The data
+processing inequality ensures post-hoc attempts to game a metric degrades both
+information content and task performance. We prove that f-mutual information
+measures are the unique gaming resistant mechanisms under natural conditions,
+with the overseer acting as an agent. While Shannon mutual information faces
+exponential sample complexity, bounded measures like total variation distance
+remain tractable. Empirically, across ten domains from translation to peer
+review, all information-theoretic mechanisms achieve perfect discrimination (d
+&gt; 0.5) between faithful and strategic agents. In contrast, LLM judges exhibit
+systematic evaluation inversion, preferring fabricated content over accurate
+summaries. Our mechanisms show 10-100x better robustness to adversarial
+manipulation than current practices. We also find performance follows an
+inverted-U curve with compression ratio, peaking at 10:1 where agent responses
+exhibit optimal information diversity (3 effective dimensions), giving a
+bias-variance perspective on when our approach is expected to be most
+effective.
 </t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>6 Pages, 9 Figures, 2 Tables</t>
+          <t>13 pages</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -778,52 +786,54 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2508.04634v1</t>
+          <t>2508.05464v1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VirtLab: An AI-Powered System for Flexible, Customizable, and
-  Large-scale Team Simulations</t>
+          <t>Bench-2-CoP: Can We Trust Benchmarking for EU AI Compliance?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mohammed Almutairi, Charles Chiang, Haoze Guo, Matthew Belcher, Nandini Banerjee, Maria Milkowski, Svitlana Volkova, Daniel Nguyen, Tim Weninger, Michael Yankoski, Trenton W. Ford, Diego Gomez-Zara</t>
+          <t>Matteo Prandi, Vincenzo Suriani, Federico Pierucci, Marcello Galisai, Daniele Nardi, Piercosma Bisconti</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>http://arxiv.org/abs/2508.04634v1</t>
+          <t>http://arxiv.org/abs/2508.05464v1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Simulating how team members collaborate within complex environments using
-Agentic AI is a promising approach to explore hypotheses grounded in social
-science theories and study team behaviors. We introduce VirtLab, a
-user-friendly, customizable, multi-agent, and scalable team simulation system
-that enables testing teams with LLM-based agents in spatial and temporal
-settings. This system addresses the current frameworks' design and technical
-limitations that do not consider flexible simulation scenarios and spatial
-settings. VirtLab contains a simulation engine and a web interface that enables
-both technical and non-technical users to formulate, run, and analyze team
-simulations without programming. We demonstrate the system's utility by
-comparing ground truth data with simulated scenarios.
+          <t xml:space="preserve">  The rapid advancement of General Purpose AI (GPAI) models necessitates robust
+evaluation frameworks, especially with emerging regulations like the EU AI Act
+and its associated Code of Practice (CoP). Current AI evaluation practices
+depend heavily on established benchmarks, but these tools were not designed to
+measure the systemic risks that are the focus of the new regulatory landscape.
+This research addresses the urgent need to quantify this "benchmark-regulation
+gap." We introduce Bench-2-CoP, a novel, systematic framework that uses
+validated LLM-as-judge analysis to map the coverage of 194,955 questions from
+widely-used benchmarks against the EU AI Act's taxonomy of model capabilities
+and propensities. Our findings reveal a profound misalignment: the evaluation
+ecosystem is overwhelmingly focused on a narrow set of behavioral propensities,
+such as "Tendency to hallucinate" (53.7% of the corpus) and "Discriminatory
+bias" (28.9%), while critical functional capabilities are dangerously
+neglected. Crucially, capabilities central to loss-of-control scenarios,
+including evading human oversight, self-replication, and autonomous AI
+development, receive zero coverage in the entire benchmark corpus. This
+translates to a near-total evaluation gap for systemic risks like "Loss of
+Control" (0.4% coverage) and "Cyber Offence" (0.8% coverage). This study
+provides the first comprehensive, quantitative analysis of this gap, offering
+critical insights for policymakers to refine the CoP and for developers to
+build the next generation of evaluation tools, ultimately fostering safer and
+more compliant AI.
 </t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>5 pages, 2 figures, UIST 2025</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>10.1145/3746058.3758994</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>Not available</t>

</xml_diff>